<commit_message>
added team retro for tic tac toe game
</commit_message>
<xml_diff>
--- a/Artifacts/Team Meeting Log.xlsx
+++ b/Artifacts/Team Meeting Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cnkeng/Desktop/fall 2020 classes/Software Design/Software-Design/Artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32D7A21-4BB5-1E45-A996-49DE21AD486C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A8007C-F2DC-AB4E-9762-4975A4156CD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-51200" yWindow="-20120" windowWidth="51200" windowHeight="28340" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
   </bookViews>
@@ -843,7 +843,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K14" sqref="K14"/>
+      <selection pane="topRight" activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1637,7 +1637,7 @@
       <c r="AW14" s="6"/>
       <c r="AX14" s="6"/>
     </row>
-    <row r="15" spans="1:50" s="8" customFormat="1" ht="210" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:50" s="8" customFormat="1" ht="112" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
retro revised and meeting log updated
</commit_message>
<xml_diff>
--- a/Artifacts/Team Meeting Log.xlsx
+++ b/Artifacts/Team Meeting Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cnkeng/Desktop/fall 2020 classes/Software Design/Software-Design/Artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A373CAF-8ACF-9244-9CBD-063E720C5A30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB49C0C-F6E8-D14A-8834-4AC17DD96F28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="74">
   <si>
     <t>Contact Info</t>
   </si>
@@ -188,9 +188,6 @@
     <t>Repeat of yesterday's meeting for those who couldn't attend</t>
   </si>
   <si>
-    <t>28m</t>
-  </si>
-  <si>
     <t>Discuss Tic-Tac-Toe game: planning, roles, timeline</t>
   </si>
   <si>
@@ -209,9 +206,6 @@
     <t>optional/spontaneous meetings</t>
   </si>
   <si>
-    <t>30m</t>
-  </si>
-  <si>
     <t>We tried to fix some GitHub branching issues, and we made it a learning experience regarding pull requests, cloning/forking, and merging.</t>
   </si>
   <si>
@@ -258,6 +252,16 @@
   </si>
   <si>
     <t>We will review the team retro during next Sunday's meeting and add anything else that comes to mind.</t>
+  </si>
+  <si>
+    <t>1 -&gt; Retro slide is finished and speaking points are assigned
+2 -&gt; Updates unknown; Ever not in meeting
+3 -&gt; Will do after meeting</t>
+  </si>
+  <si>
+    <t>1 -&gt; Retro Revision (decide who's presenting which slide, summarize the slides and make it less wordy)
+2 -&gt; Prof. Vallone's feedback (status update from Ever: did you create Jira issues for it?)
+3 -&gt; Reminder for everyone to go over the tic-tac-toe implementation project Prof. Vallone sent us</t>
   </si>
 </sst>
 </file>
@@ -365,12 +369,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -385,6 +383,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
   </fills>
@@ -410,7 +414,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -471,9 +475,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -496,16 +497,16 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -528,6 +529,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -850,9 +855,9 @@
   </sheetPr>
   <dimension ref="A1:AX24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="118" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -869,85 +874,86 @@
     <col min="12" max="12" width="24.33203125" customWidth="1"/>
     <col min="13" max="13" width="21" customWidth="1"/>
     <col min="14" max="14" width="20.1640625" customWidth="1"/>
-    <col min="15" max="20" width="11" customWidth="1"/>
+    <col min="15" max="15" width="26.83203125" customWidth="1"/>
+    <col min="16" max="20" width="11" customWidth="1"/>
     <col min="21" max="31" width="12.6640625" customWidth="1"/>
     <col min="32" max="36" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
       <c r="J1" s="26"/>
       <c r="K1" s="26"/>
     </row>
     <row r="2" spans="1:50" s="23" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49" t="s">
+      <c r="C2" s="48"/>
+      <c r="D2" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
       <c r="Q2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="45" t="s">
+      <c r="R2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="45"/>
-      <c r="T2" s="45"/>
-      <c r="U2" s="45"/>
-      <c r="V2" s="45"/>
-      <c r="W2" s="45"/>
-      <c r="X2" s="45" t="s">
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
+      <c r="V2" s="44"/>
+      <c r="W2" s="44"/>
+      <c r="X2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="Y2" s="45"/>
-      <c r="Z2" s="45"/>
-      <c r="AA2" s="45"/>
-      <c r="AB2" s="45"/>
-      <c r="AC2" s="45"/>
-      <c r="AD2" s="45" t="s">
+      <c r="Y2" s="44"/>
+      <c r="Z2" s="44"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="AE2" s="45"/>
-      <c r="AF2" s="45"/>
-      <c r="AG2" s="45"/>
-      <c r="AH2" s="45"/>
-      <c r="AI2" s="45"/>
-      <c r="AJ2" s="45"/>
-      <c r="AK2" s="45" t="s">
+      <c r="AE2" s="44"/>
+      <c r="AF2" s="44"/>
+      <c r="AG2" s="44"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="AL2" s="45"/>
-      <c r="AM2" s="45"/>
-      <c r="AN2" s="45"/>
-      <c r="AO2" s="45"/>
-      <c r="AP2" s="45"/>
-      <c r="AQ2" s="33"/>
-      <c r="AR2" s="33"/>
-      <c r="AS2" s="33"/>
-      <c r="AT2" s="33"/>
-      <c r="AU2" s="33"/>
+      <c r="AL2" s="44"/>
+      <c r="AM2" s="44"/>
+      <c r="AN2" s="44"/>
+      <c r="AO2" s="44"/>
+      <c r="AP2" s="44"/>
+      <c r="AQ2" s="32"/>
+      <c r="AR2" s="32"/>
+      <c r="AS2" s="32"/>
+      <c r="AT2" s="32"/>
+      <c r="AU2" s="32"/>
       <c r="AV2" s="22"/>
       <c r="AW2" s="22"/>
       <c r="AX2" s="22"/>
@@ -962,128 +968,128 @@
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="30">
         <v>44066</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="30">
         <v>44067</v>
       </c>
-      <c r="F3" s="31">
+      <c r="F3" s="30">
         <v>44068</v>
       </c>
-      <c r="G3" s="31">
+      <c r="G3" s="30">
         <v>44073</v>
       </c>
-      <c r="H3" s="31">
+      <c r="H3" s="30">
         <v>44074</v>
       </c>
-      <c r="I3" s="31">
+      <c r="I3" s="30">
         <v>44075</v>
       </c>
-      <c r="J3" s="42">
+      <c r="J3" s="41">
         <v>44078</v>
       </c>
-      <c r="K3" s="42">
+      <c r="K3" s="41">
         <v>44079</v>
       </c>
-      <c r="L3" s="31">
+      <c r="L3" s="30">
         <v>44080</v>
       </c>
-      <c r="M3" s="31">
+      <c r="M3" s="30">
         <v>44081</v>
       </c>
-      <c r="N3" s="31">
+      <c r="N3" s="30">
         <v>44082</v>
       </c>
-      <c r="O3" s="31">
+      <c r="O3" s="30">
         <v>44087</v>
       </c>
-      <c r="P3" s="31">
+      <c r="P3" s="30">
         <v>44088</v>
       </c>
-      <c r="Q3" s="31">
+      <c r="Q3" s="30">
         <v>44089</v>
       </c>
-      <c r="R3" s="31">
+      <c r="R3" s="30">
         <v>44094</v>
       </c>
-      <c r="S3" s="31">
+      <c r="S3" s="30">
         <v>44095</v>
       </c>
-      <c r="T3" s="31">
+      <c r="T3" s="30">
         <v>44096</v>
       </c>
-      <c r="U3" s="31">
+      <c r="U3" s="30">
         <v>44101</v>
       </c>
-      <c r="V3" s="31">
+      <c r="V3" s="30">
         <v>44102</v>
       </c>
-      <c r="W3" s="31">
+      <c r="W3" s="30">
         <v>44103</v>
       </c>
-      <c r="X3" s="31">
+      <c r="X3" s="30">
         <v>44108</v>
       </c>
-      <c r="Y3" s="31">
+      <c r="Y3" s="30">
         <v>44109</v>
       </c>
-      <c r="Z3" s="31">
+      <c r="Z3" s="30">
         <v>44110</v>
       </c>
-      <c r="AA3" s="31">
+      <c r="AA3" s="30">
         <v>44115</v>
       </c>
-      <c r="AB3" s="31">
+      <c r="AB3" s="30">
         <v>44116</v>
       </c>
-      <c r="AC3" s="31">
+      <c r="AC3" s="30">
         <v>44117</v>
       </c>
-      <c r="AD3" s="31">
+      <c r="AD3" s="30">
         <v>44122</v>
       </c>
-      <c r="AE3" s="31">
+      <c r="AE3" s="30">
         <v>44123</v>
       </c>
-      <c r="AF3" s="31">
+      <c r="AF3" s="30">
         <v>44124</v>
       </c>
-      <c r="AG3" s="31">
+      <c r="AG3" s="30">
         <v>44129</v>
       </c>
-      <c r="AH3" s="31">
+      <c r="AH3" s="30">
         <v>44130</v>
       </c>
-      <c r="AI3" s="31">
+      <c r="AI3" s="30">
         <v>44131</v>
       </c>
-      <c r="AJ3" s="31">
+      <c r="AJ3" s="30">
         <v>44136</v>
       </c>
-      <c r="AK3" s="31">
+      <c r="AK3" s="30">
         <v>44137</v>
       </c>
-      <c r="AL3" s="31">
+      <c r="AL3" s="30">
         <v>44138</v>
       </c>
-      <c r="AM3" s="31">
+      <c r="AM3" s="30">
         <v>44143</v>
       </c>
-      <c r="AN3" s="32">
+      <c r="AN3" s="31">
         <v>44144</v>
       </c>
-      <c r="AO3" s="32">
+      <c r="AO3" s="31">
         <v>44145</v>
       </c>
-      <c r="AP3" s="31">
+      <c r="AP3" s="30">
         <v>44150</v>
       </c>
-      <c r="AQ3" s="34"/>
-      <c r="AR3" s="34"/>
-      <c r="AS3" s="34"/>
-      <c r="AT3" s="34"/>
-      <c r="AU3" s="34"/>
+      <c r="AQ3" s="33"/>
+      <c r="AR3" s="33"/>
+      <c r="AS3" s="33"/>
+      <c r="AT3" s="33"/>
+      <c r="AU3" s="33"/>
       <c r="AV3" s="13"/>
       <c r="AW3" s="13"/>
       <c r="AX3" s="13"/>
@@ -1131,7 +1137,9 @@
       <c r="N4" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="28"/>
+      <c r="O4" s="28" t="s">
+        <v>9</v>
+      </c>
       <c r="P4" s="28"/>
       <c r="Q4" s="28"/>
       <c r="R4" s="28"/>
@@ -1174,15 +1182,15 @@
       <c r="F5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="30"/>
+      <c r="G5" s="42"/>
       <c r="H5" s="28" t="s">
         <v>9</v>
       </c>
       <c r="I5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
       <c r="L5" s="27" t="s">
         <v>9</v>
       </c>
@@ -1192,7 +1200,7 @@
       <c r="N5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="28"/>
+      <c r="O5" s="42"/>
       <c r="P5" s="28"/>
       <c r="Q5" s="28"/>
       <c r="R5" s="28"/>
@@ -1229,7 +1237,7 @@
       <c r="D6" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="30"/>
+      <c r="E6" s="50"/>
       <c r="F6" s="28" t="s">
         <v>9</v>
       </c>
@@ -1239,8 +1247,8 @@
       <c r="H6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="30"/>
-      <c r="J6" s="39"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="38"/>
       <c r="K6" s="28" t="s">
         <v>9</v>
       </c>
@@ -1253,7 +1261,7 @@
       <c r="N6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="O6" s="28"/>
+      <c r="O6" s="50"/>
       <c r="P6" s="28"/>
       <c r="Q6" s="28"/>
       <c r="R6" s="28"/>
@@ -1290,21 +1298,21 @@
       <c r="D7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="42" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="30"/>
+      <c r="G7" s="42"/>
       <c r="H7" s="28" t="s">
         <v>9</v>
       </c>
       <c r="I7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
       <c r="L7" s="27" t="s">
         <v>9</v>
       </c>
@@ -1314,7 +1322,7 @@
       <c r="N7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="28"/>
+      <c r="O7" s="42"/>
       <c r="P7" s="28"/>
       <c r="Q7" s="28"/>
       <c r="R7" s="28"/>
@@ -1360,22 +1368,24 @@
       <c r="G8" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="30"/>
+      <c r="H8" s="42"/>
       <c r="I8" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="39"/>
+      <c r="J8" s="38"/>
       <c r="K8" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="L8" s="30"/>
+      <c r="L8" s="42"/>
       <c r="M8" s="27" t="s">
         <v>9</v>
       </c>
       <c r="N8" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="O8" s="28"/>
+      <c r="O8" s="28" t="s">
+        <v>9</v>
+      </c>
       <c r="P8" s="28"/>
       <c r="Q8" s="28"/>
       <c r="R8" s="28"/>
@@ -1424,7 +1434,7 @@
       <c r="H9" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="30"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="28" t="s">
         <v>9</v>
       </c>
@@ -1434,11 +1444,13 @@
       <c r="L9" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="30"/>
+      <c r="M9" s="42"/>
       <c r="N9" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="28"/>
+      <c r="O9" s="28" t="s">
+        <v>9</v>
+      </c>
       <c r="P9" s="28"/>
       <c r="Q9" s="28"/>
       <c r="R9" s="28"/>
@@ -1475,7 +1487,7 @@
       <c r="D10" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="42" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="28" t="s">
@@ -1484,14 +1496,14 @@
       <c r="G10" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="43" t="s">
+      <c r="H10" s="42" t="s">
         <v>10</v>
       </c>
       <c r="I10" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
       <c r="L10" s="27" t="s">
         <v>9</v>
       </c>
@@ -1501,7 +1513,9 @@
       <c r="N10" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="28"/>
+      <c r="O10" s="28" t="s">
+        <v>9</v>
+      </c>
       <c r="P10" s="28"/>
       <c r="Q10" s="28"/>
       <c r="R10" s="28"/>
@@ -1526,10 +1540,10 @@
       <c r="AK10" s="29"/>
     </row>
     <row r="11" spans="1:50" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-    </row>
-    <row r="13" spans="1:50" ht="124" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+    </row>
+    <row r="13" spans="1:50" ht="185" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -1549,7 +1563,7 @@
         <v>49</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>41</v>
@@ -1557,16 +1571,18 @@
       <c r="K13" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="L13" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="M13" s="36" t="s">
-        <v>67</v>
+      <c r="L13" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="M13" s="35" t="s">
+        <v>65</v>
       </c>
       <c r="N13" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="O13" s="18"/>
+        <v>70</v>
+      </c>
+      <c r="O13" s="18" t="s">
+        <v>73</v>
+      </c>
       <c r="P13" s="18"/>
       <c r="Q13" s="18"/>
       <c r="R13" s="18"/>
@@ -1605,30 +1621,32 @@
         <v>47</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J14" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="K14" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="L14" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="M14" s="35" t="s">
+      <c r="L14" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="M14" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="N14" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="N14" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="O14" s="19"/>
+      <c r="O14" s="19" t="s">
+        <v>72</v>
+      </c>
       <c r="P14" s="19"/>
       <c r="Q14" s="19"/>
       <c r="R14" s="19"/>
@@ -1647,8 +1665,8 @@
       <c r="AE14" s="19"/>
       <c r="AF14" s="19"/>
       <c r="AG14" s="19"/>
-      <c r="AH14" s="46"/>
-      <c r="AI14" s="47"/>
+      <c r="AH14" s="45"/>
+      <c r="AI14" s="46"/>
       <c r="AJ14" s="19"/>
       <c r="AK14" s="19"/>
       <c r="AL14" s="6"/>
@@ -1671,7 +1689,7 @@
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>41</v>
@@ -1680,30 +1698,32 @@
         <v>44</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H15" s="19" t="s">
         <v>41</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J15" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="K15" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="K15" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="L15" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="M15" s="35" t="s">
+      <c r="L15" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="M15" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="N15" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="O15" s="19"/>
+      <c r="N15" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="O15" s="19" t="s">
+        <v>41</v>
+      </c>
       <c r="P15" s="19"/>
       <c r="Q15" s="19"/>
       <c r="R15" s="19"/>
@@ -1750,56 +1770,62 @@
       <c r="E16" s="20">
         <v>3</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="20">
         <v>30</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="20">
         <v>5</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="20">
         <v>5</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="I16" s="20">
+        <v>28</v>
+      </c>
+      <c r="J16" s="20">
+        <v>30</v>
+      </c>
+      <c r="K16" s="20">
+        <v>30</v>
+      </c>
+      <c r="L16" s="20">
+        <v>17</v>
+      </c>
+      <c r="M16" s="20">
         <v>50</v>
       </c>
-      <c r="J16" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="K16" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="L16" s="36">
-        <v>17</v>
-      </c>
-      <c r="M16" s="36">
-        <v>50</v>
-      </c>
-      <c r="N16" s="18">
+      <c r="N16" s="20">
         <v>55</v>
       </c>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
-      <c r="T16" s="18"/>
-      <c r="U16" s="18"/>
-      <c r="V16" s="18"/>
-      <c r="W16" s="18"/>
-      <c r="X16" s="18"/>
-      <c r="Y16" s="18"/>
-      <c r="Z16" s="18"/>
-      <c r="AA16" s="18"/>
-      <c r="AB16" s="18"/>
-      <c r="AC16" s="18"/>
-      <c r="AD16" s="18"/>
-      <c r="AE16" s="18"/>
-      <c r="AF16" s="18"/>
-      <c r="AG16" s="18"/>
-      <c r="AH16" s="18"/>
-      <c r="AI16" s="18"/>
-      <c r="AJ16" s="18"/>
-      <c r="AK16" s="18"/>
+      <c r="O16" s="20">
+        <v>30</v>
+      </c>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="20"/>
+      <c r="U16" s="20"/>
+      <c r="V16" s="20"/>
+      <c r="W16" s="20"/>
+      <c r="X16" s="20"/>
+      <c r="Y16" s="20"/>
+      <c r="Z16" s="20"/>
+      <c r="AA16" s="20"/>
+      <c r="AB16" s="20"/>
+      <c r="AC16" s="20"/>
+      <c r="AD16" s="20"/>
+      <c r="AE16" s="20"/>
+      <c r="AF16" s="20"/>
+      <c r="AG16" s="20"/>
+      <c r="AH16" s="20"/>
+      <c r="AI16" s="20"/>
+      <c r="AJ16" s="20"/>
+      <c r="AK16" s="20"/>
+      <c r="AL16" s="49"/>
+      <c r="AM16" s="49"/>
+      <c r="AN16" s="49"/>
+      <c r="AO16" s="49"/>
     </row>
     <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="3"/>
@@ -1815,8 +1841,8 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="28" x14ac:dyDescent="0.15">
-      <c r="B20" s="41" t="s">
-        <v>56</v>
+      <c r="B20" s="40" t="s">
+        <v>55</v>
       </c>
       <c r="C20" s="15"/>
     </row>
@@ -1826,14 +1852,14 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="42" x14ac:dyDescent="0.15">
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="37" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="15"/>
     </row>
     <row r="23" spans="1:21" ht="46" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="40" t="s">
-        <v>59</v>
+      <c r="B23" s="39" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="13" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
updated meeting log and added coding standards doc
</commit_message>
<xml_diff>
--- a/Artifacts/Team Meeting Log.xlsx
+++ b/Artifacts/Team Meeting Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cnkeng/Desktop/fall 2020 classes/Software Design/Software-Design/Artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B296E1F9-0293-9947-AD2B-FBB092738E48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E0CAB6-7856-1C49-9252-EC490E941A88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9100" yWindow="-28340" windowWidth="51200" windowHeight="26880" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
+    <workbookView xWindow="-7660" yWindow="-28340" windowWidth="51200" windowHeight="28340" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
   </bookViews>
   <sheets>
     <sheet name="TeamF" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="81">
   <si>
     <t>Contact Info</t>
   </si>
@@ -277,6 +277,12 @@
   </si>
   <si>
     <t>We added additional bullets to each section and we assigned speaking points for each teammate.</t>
+  </si>
+  <si>
+    <t>Think of additional items for Coding Standards &amp; Guidelines for tomorrow's meeting.</t>
+  </si>
+  <si>
+    <t>We explored different ideas and came up with a brief document, outlining our team's coding standards and guidelines. We plan to apply these guidelines to all of our future coding projects.</t>
   </si>
 </sst>
 </file>
@@ -558,6 +564,9 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -572,9 +581,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -898,8 +904,8 @@
   <dimension ref="A1:AX24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M14" sqref="M14"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -918,81 +924,82 @@
     <col min="14" max="14" width="20.1640625" customWidth="1"/>
     <col min="15" max="15" width="26.83203125" customWidth="1"/>
     <col min="16" max="17" width="18.83203125" customWidth="1"/>
-    <col min="18" max="18" width="17.6640625" customWidth="1"/>
-    <col min="19" max="21" width="11" customWidth="1"/>
+    <col min="18" max="18" width="20.33203125" customWidth="1"/>
+    <col min="19" max="19" width="19.5" customWidth="1"/>
+    <col min="20" max="21" width="11" customWidth="1"/>
     <col min="22" max="32" width="12.6640625" customWidth="1"/>
     <col min="33" max="37" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
       <c r="J1" s="26"/>
       <c r="K1" s="26"/>
     </row>
     <row r="2" spans="1:50" s="23" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54" t="s">
+      <c r="C2" s="55"/>
+      <c r="D2" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54" t="s">
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
       <c r="R2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="50" t="s">
+      <c r="S2" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
-      <c r="W2" s="50"/>
-      <c r="X2" s="50"/>
-      <c r="Y2" s="50" t="s">
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="51"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="50"/>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="50"/>
-      <c r="AC2" s="50"/>
-      <c r="AD2" s="50"/>
-      <c r="AE2" s="50" t="s">
+      <c r="Z2" s="51"/>
+      <c r="AA2" s="51"/>
+      <c r="AB2" s="51"/>
+      <c r="AC2" s="51"/>
+      <c r="AD2" s="51"/>
+      <c r="AE2" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="AF2" s="50"/>
-      <c r="AG2" s="50"/>
-      <c r="AH2" s="50"/>
-      <c r="AI2" s="50"/>
-      <c r="AJ2" s="50"/>
-      <c r="AK2" s="50"/>
-      <c r="AL2" s="50" t="s">
+      <c r="AF2" s="51"/>
+      <c r="AG2" s="51"/>
+      <c r="AH2" s="51"/>
+      <c r="AI2" s="51"/>
+      <c r="AJ2" s="51"/>
+      <c r="AK2" s="51"/>
+      <c r="AL2" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="AM2" s="50"/>
-      <c r="AN2" s="50"/>
-      <c r="AO2" s="50"/>
-      <c r="AP2" s="50"/>
+      <c r="AM2" s="51"/>
+      <c r="AN2" s="51"/>
+      <c r="AO2" s="51"/>
+      <c r="AP2" s="51"/>
       <c r="AQ2" s="32"/>
       <c r="AR2" s="32"/>
       <c r="AS2" s="32"/>
@@ -1190,7 +1197,9 @@
       <c r="Q4" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="28"/>
+      <c r="R4" s="28" t="s">
+        <v>9</v>
+      </c>
       <c r="S4" s="28"/>
       <c r="T4" s="28"/>
       <c r="U4" s="28"/>
@@ -1254,7 +1263,9 @@
       <c r="Q5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="R5" s="28"/>
+      <c r="R5" s="28" t="s">
+        <v>9</v>
+      </c>
       <c r="S5" s="28"/>
       <c r="T5" s="28"/>
       <c r="U5" s="28"/>
@@ -1320,7 +1331,7 @@
       <c r="Q6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="R6" s="28"/>
+      <c r="R6" s="49"/>
       <c r="S6" s="28"/>
       <c r="T6" s="28"/>
       <c r="U6" s="28"/>
@@ -1386,7 +1397,7 @@
       <c r="Q7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="R7" s="28"/>
+      <c r="R7" s="49"/>
       <c r="S7" s="28"/>
       <c r="T7" s="28"/>
       <c r="U7" s="28"/>
@@ -1454,7 +1465,9 @@
       <c r="Q8" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="R8" s="28"/>
+      <c r="R8" s="28" t="s">
+        <v>9</v>
+      </c>
       <c r="S8" s="28"/>
       <c r="T8" s="28"/>
       <c r="U8" s="28"/>
@@ -1522,7 +1535,9 @@
         <v>9</v>
       </c>
       <c r="Q9" s="49"/>
-      <c r="R9" s="28"/>
+      <c r="R9" s="28" t="s">
+        <v>9</v>
+      </c>
       <c r="S9" s="28"/>
       <c r="T9" s="28"/>
       <c r="U9" s="28"/>
@@ -1587,10 +1602,12 @@
         <v>9</v>
       </c>
       <c r="P10" s="48"/>
-      <c r="Q10" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="R10" s="28"/>
+      <c r="Q10" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="R10" s="28" t="s">
+        <v>9</v>
+      </c>
       <c r="S10" s="28"/>
       <c r="T10" s="28"/>
       <c r="U10" s="28"/>
@@ -1734,7 +1751,9 @@
       <c r="Q14" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="R14" s="19"/>
+      <c r="R14" s="19" t="s">
+        <v>80</v>
+      </c>
       <c r="S14" s="19"/>
       <c r="T14" s="19"/>
       <c r="U14" s="19"/>
@@ -1751,8 +1770,8 @@
       <c r="AF14" s="19"/>
       <c r="AG14" s="19"/>
       <c r="AH14" s="19"/>
-      <c r="AI14" s="51"/>
-      <c r="AJ14" s="52"/>
+      <c r="AI14" s="52"/>
+      <c r="AJ14" s="53"/>
       <c r="AK14" s="19"/>
       <c r="AL14" s="19"/>
       <c r="AM14" s="6"/>
@@ -1815,7 +1834,9 @@
       <c r="Q15" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="R15" s="19"/>
+      <c r="R15" s="19" t="s">
+        <v>79</v>
+      </c>
       <c r="S15" s="19"/>
       <c r="T15" s="19"/>
       <c r="U15" s="19"/>
@@ -1895,7 +1916,9 @@
       <c r="Q16" s="20">
         <v>20</v>
       </c>
-      <c r="R16" s="20"/>
+      <c r="R16" s="20">
+        <v>35</v>
+      </c>
       <c r="S16" s="20"/>
       <c r="T16" s="20"/>
       <c r="U16" s="20"/>

</xml_diff>

<commit_message>
edited the action items for tomorro'w meeting
</commit_message>
<xml_diff>
--- a/Artifacts/Team Meeting Log.xlsx
+++ b/Artifacts/Team Meeting Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cnkeng/Desktop/fall 2020 classes/Software Design/Software-Design/Artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E0CAB6-7856-1C49-9252-EC490E941A88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA19432-F3D3-5241-8941-961EC6A2BF4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-7660" yWindow="-28340" windowWidth="51200" windowHeight="28340" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
   </bookViews>
@@ -279,10 +279,10 @@
     <t>We added additional bullets to each section and we assigned speaking points for each teammate.</t>
   </si>
   <si>
-    <t>Think of additional items for Coding Standards &amp; Guidelines for tomorrow's meeting.</t>
-  </si>
-  <si>
     <t>We explored different ideas and came up with a brief document, outlining our team's coding standards and guidelines. We plan to apply these guidelines to all of our future coding projects.</t>
+  </si>
+  <si>
+    <t>Everyone must come up with at least 3 additional items for Coding Standards &amp; Guidelines doc for tomorrow's meeting.</t>
   </si>
 </sst>
 </file>
@@ -905,7 +905,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
       <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U14" sqref="U14"/>
+      <selection pane="topRight" activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1752,7 +1752,7 @@
         <v>78</v>
       </c>
       <c r="R14" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S14" s="19"/>
       <c r="T14" s="19"/>
@@ -1835,7 +1835,7 @@
         <v>41</v>
       </c>
       <c r="R15" s="19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="S15" s="19"/>
       <c r="T15" s="19"/>

</xml_diff>

<commit_message>
revised guidelines and updated attendance
</commit_message>
<xml_diff>
--- a/Artifacts/Team Meeting Log.xlsx
+++ b/Artifacts/Team Meeting Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cnkeng/Desktop/fall 2020 classes/Software Design/Software-Design/Artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA19432-F3D3-5241-8941-961EC6A2BF4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171D0299-2B48-C04C-A3FA-25C93978E010}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-7660" yWindow="-28340" windowWidth="51200" windowHeight="28340" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="83">
   <si>
     <t>Contact Info</t>
   </si>
@@ -283,6 +283,12 @@
   </si>
   <si>
     <t>Everyone must come up with at least 3 additional items for Coding Standards &amp; Guidelines doc for tomorrow's meeting.</t>
+  </si>
+  <si>
+    <t>Revise the Coding Standards &amp; Guidelines document.</t>
+  </si>
+  <si>
+    <t>We added more items to our team doc and updated it in the repo.</t>
   </si>
 </sst>
 </file>
@@ -904,8 +910,8 @@
   <dimension ref="A1:AX24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S15" sqref="S15"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1200,7 +1206,9 @@
       <c r="R4" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="28"/>
+      <c r="S4" s="28" t="s">
+        <v>9</v>
+      </c>
       <c r="T4" s="28"/>
       <c r="U4" s="28"/>
       <c r="V4" s="28"/>
@@ -1266,7 +1274,7 @@
       <c r="R5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="S5" s="28"/>
+      <c r="S5" s="49"/>
       <c r="T5" s="28"/>
       <c r="U5" s="28"/>
       <c r="V5" s="28"/>
@@ -1332,7 +1340,9 @@
         <v>9</v>
       </c>
       <c r="R6" s="49"/>
-      <c r="S6" s="28"/>
+      <c r="S6" s="28" t="s">
+        <v>9</v>
+      </c>
       <c r="T6" s="28"/>
       <c r="U6" s="28"/>
       <c r="V6" s="28"/>
@@ -1398,7 +1408,9 @@
         <v>9</v>
       </c>
       <c r="R7" s="49"/>
-      <c r="S7" s="28"/>
+      <c r="S7" s="28" t="s">
+        <v>9</v>
+      </c>
       <c r="T7" s="28"/>
       <c r="U7" s="28"/>
       <c r="V7" s="28"/>
@@ -1468,7 +1480,7 @@
       <c r="R8" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="S8" s="28"/>
+      <c r="S8" s="42"/>
       <c r="T8" s="28"/>
       <c r="U8" s="28"/>
       <c r="V8" s="28"/>
@@ -1538,7 +1550,9 @@
       <c r="R9" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="S9" s="28"/>
+      <c r="S9" s="28" t="s">
+        <v>9</v>
+      </c>
       <c r="T9" s="28"/>
       <c r="U9" s="28"/>
       <c r="V9" s="28"/>
@@ -1608,7 +1622,7 @@
       <c r="R10" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="S10" s="28"/>
+      <c r="S10" s="42"/>
       <c r="T10" s="28"/>
       <c r="U10" s="28"/>
       <c r="V10" s="28"/>
@@ -1683,7 +1697,9 @@
       <c r="R13" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="S13" s="18"/>
+      <c r="S13" s="18" t="s">
+        <v>81</v>
+      </c>
       <c r="T13" s="18"/>
       <c r="U13" s="18"/>
       <c r="V13" s="18"/>
@@ -1754,7 +1770,9 @@
       <c r="R14" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="S14" s="19"/>
+      <c r="S14" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="T14" s="19"/>
       <c r="U14" s="19"/>
       <c r="V14" s="19"/>
@@ -1837,7 +1855,9 @@
       <c r="R15" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="S15" s="19"/>
+      <c r="S15" s="19" t="s">
+        <v>41</v>
+      </c>
       <c r="T15" s="19"/>
       <c r="U15" s="19"/>
       <c r="V15" s="19"/>
@@ -1919,7 +1939,9 @@
       <c r="R16" s="20">
         <v>35</v>
       </c>
-      <c r="S16" s="20"/>
+      <c r="S16" s="20">
+        <v>17</v>
+      </c>
       <c r="T16" s="20"/>
       <c r="U16" s="20"/>
       <c r="V16" s="20"/>

</xml_diff>

<commit_message>
uploaded required docs and updated team meeting log
</commit_message>
<xml_diff>
--- a/Artifacts/Team Meeting Log.xlsx
+++ b/Artifacts/Team Meeting Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cnkeng/Desktop/fall 2020 classes/Software Design/Software-Design/Artifacts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cnken\Desktop\Software-Design\Artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378232C0-5363-494C-B396-3D9DAFD95B7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBE460B-830A-4B27-A117-50E0AE3648C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7660" yWindow="-28340" windowWidth="51200" windowHeight="28340" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
   </bookViews>
   <sheets>
     <sheet name="TeamF" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="85">
   <si>
     <t>Contact Info</t>
   </si>
@@ -286,6 +286,15 @@
   </si>
   <si>
     <t>We added more items to our team doc and updated it in the repo.</t>
+  </si>
+  <si>
+    <t>Go over Timeline, Tools doc, and Requirements doc</t>
+  </si>
+  <si>
+    <t>We created a project timeline, revisited our Tools document, and created our Project Requirements.</t>
+  </si>
+  <si>
+    <t>Get the Jira workspace set up</t>
   </si>
 </sst>
 </file>
@@ -924,35 +933,36 @@
   </sheetPr>
   <dimension ref="A1:AX24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X7" sqref="X7:X8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.1328125" customWidth="1"/>
+    <col min="4" max="4" width="25.796875" customWidth="1"/>
+    <col min="5" max="5" width="17.46484375" customWidth="1"/>
+    <col min="6" max="6" width="16.46484375" customWidth="1"/>
+    <col min="7" max="7" width="18.1328125" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" customWidth="1"/>
-    <col min="9" max="11" width="25.1640625" customWidth="1"/>
+    <col min="9" max="11" width="25.1328125" customWidth="1"/>
     <col min="12" max="12" width="24.33203125" customWidth="1"/>
     <col min="13" max="13" width="21" customWidth="1"/>
-    <col min="14" max="14" width="20.1640625" customWidth="1"/>
-    <col min="15" max="15" width="26.83203125" customWidth="1"/>
-    <col min="16" max="17" width="18.83203125" customWidth="1"/>
+    <col min="14" max="14" width="20.1328125" customWidth="1"/>
+    <col min="15" max="15" width="26.796875" customWidth="1"/>
+    <col min="16" max="17" width="18.796875" customWidth="1"/>
     <col min="18" max="18" width="20.33203125" customWidth="1"/>
-    <col min="19" max="19" width="19.5" customWidth="1"/>
-    <col min="20" max="21" width="11" customWidth="1"/>
+    <col min="19" max="19" width="19.46484375" customWidth="1"/>
+    <col min="20" max="20" width="18" customWidth="1"/>
+    <col min="21" max="21" width="11" customWidth="1"/>
     <col min="22" max="32" width="12.6640625" customWidth="1"/>
     <col min="33" max="37" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="E1" s="54" t="s">
         <v>36</v>
       </c>
@@ -963,7 +973,7 @@
       <c r="J1" s="26"/>
       <c r="K1" s="26"/>
     </row>
-    <row r="2" spans="1:50" s="23" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:50" s="23" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
@@ -1028,7 +1038,7 @@
       <c r="AW2" s="22"/>
       <c r="AX2" s="22"/>
     </row>
-    <row r="3" spans="1:50" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:50" s="1" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
@@ -1164,7 +1174,7 @@
       <c r="AW3" s="13"/>
       <c r="AX3" s="13"/>
     </row>
-    <row r="4" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:50" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>15</v>
       </c>
@@ -1222,7 +1232,9 @@
       <c r="S4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="T4" s="28"/>
+      <c r="T4" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="U4" s="28"/>
       <c r="V4" s="28"/>
       <c r="W4" s="28"/>
@@ -1242,7 +1254,7 @@
       <c r="AK4" s="28"/>
       <c r="AL4" s="29"/>
     </row>
-    <row r="5" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:50" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>16</v>
       </c>
@@ -1288,7 +1300,9 @@
         <v>8</v>
       </c>
       <c r="S5" s="49"/>
-      <c r="T5" s="28"/>
+      <c r="T5" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="U5" s="28"/>
       <c r="V5" s="28"/>
       <c r="W5" s="28"/>
@@ -1308,7 +1322,7 @@
       <c r="AK5" s="28"/>
       <c r="AL5" s="29"/>
     </row>
-    <row r="6" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:50" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>17</v>
       </c>
@@ -1356,7 +1370,9 @@
       <c r="S6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="T6" s="28"/>
+      <c r="T6" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="U6" s="28"/>
       <c r="V6" s="28"/>
       <c r="W6" s="28"/>
@@ -1376,7 +1392,7 @@
       <c r="AK6" s="28"/>
       <c r="AL6" s="29"/>
     </row>
-    <row r="7" spans="1:50" ht="14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:50" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>18</v>
       </c>
@@ -1424,7 +1440,9 @@
       <c r="S7" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="T7" s="28"/>
+      <c r="T7" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="U7" s="28"/>
       <c r="V7" s="28"/>
       <c r="W7" s="42"/>
@@ -1444,7 +1462,7 @@
       <c r="AK7" s="28"/>
       <c r="AL7" s="29"/>
     </row>
-    <row r="8" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:50" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>20</v>
       </c>
@@ -1494,7 +1512,9 @@
         <v>8</v>
       </c>
       <c r="S8" s="42"/>
-      <c r="T8" s="28"/>
+      <c r="T8" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="U8" s="28"/>
       <c r="V8" s="28"/>
       <c r="W8" s="28"/>
@@ -1514,7 +1534,7 @@
       <c r="AK8" s="28"/>
       <c r="AL8" s="29"/>
     </row>
-    <row r="9" spans="1:50" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:50" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>21</v>
       </c>
@@ -1566,7 +1586,7 @@
       <c r="S9" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="T9" s="28"/>
+      <c r="T9" s="49"/>
       <c r="U9" s="28"/>
       <c r="V9" s="28"/>
       <c r="W9" s="28"/>
@@ -1586,7 +1606,7 @@
       <c r="AK9" s="28"/>
       <c r="AL9" s="29"/>
     </row>
-    <row r="10" spans="1:50" ht="14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:50" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>19</v>
       </c>
@@ -1636,7 +1656,9 @@
         <v>8</v>
       </c>
       <c r="S10" s="42"/>
-      <c r="T10" s="28"/>
+      <c r="T10" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="U10" s="28"/>
       <c r="V10" s="28"/>
       <c r="W10" s="28"/>
@@ -1656,12 +1678,12 @@
       <c r="AK10" s="28"/>
       <c r="AL10" s="29"/>
     </row>
-    <row r="11" spans="1:50" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:50" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J11" s="36"/>
       <c r="K11" s="36"/>
       <c r="Q11" s="36"/>
     </row>
-    <row r="13" spans="1:50" ht="185" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:50" ht="185" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>37</v>
       </c>
@@ -1713,7 +1735,9 @@
       <c r="S13" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="T13" s="18"/>
+      <c r="T13" s="18" t="s">
+        <v>82</v>
+      </c>
       <c r="U13" s="18"/>
       <c r="V13" s="18"/>
       <c r="W13" s="18"/>
@@ -1733,7 +1757,7 @@
       <c r="AK13" s="18"/>
       <c r="AL13" s="18"/>
     </row>
-    <row r="14" spans="1:50" s="5" customFormat="1" ht="259" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:50" s="5" customFormat="1" ht="259.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="14" t="s">
         <v>38</v>
       </c>
@@ -1786,7 +1810,9 @@
       <c r="S14" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="T14" s="19"/>
+      <c r="T14" s="19" t="s">
+        <v>83</v>
+      </c>
       <c r="U14" s="19"/>
       <c r="V14" s="19"/>
       <c r="W14" s="19"/>
@@ -1818,7 +1844,7 @@
       <c r="AW14" s="6"/>
       <c r="AX14" s="6"/>
     </row>
-    <row r="15" spans="1:50" s="8" customFormat="1" ht="112" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:50" s="8" customFormat="1" ht="102" x14ac:dyDescent="0.4">
       <c r="A15" s="14" t="s">
         <v>39</v>
       </c>
@@ -1871,7 +1897,9 @@
       <c r="S15" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="T15" s="19"/>
+      <c r="T15" s="19" t="s">
+        <v>84</v>
+      </c>
       <c r="U15" s="19"/>
       <c r="V15" s="19"/>
       <c r="W15" s="19"/>
@@ -1903,7 +1931,7 @@
       <c r="AW15" s="7"/>
       <c r="AX15" s="7"/>
     </row>
-    <row r="16" spans="1:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
@@ -1955,7 +1983,9 @@
       <c r="S16" s="20">
         <v>17</v>
       </c>
-      <c r="T16" s="20"/>
+      <c r="T16" s="20">
+        <v>50</v>
+      </c>
       <c r="U16" s="20"/>
       <c r="V16" s="20"/>
       <c r="W16" s="20"/>
@@ -1979,42 +2009,42 @@
       <c r="AO16" s="44"/>
       <c r="AP16" s="44"/>
     </row>
-    <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:22" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:22" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:22" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B19" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="28" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:22" ht="25.5" x14ac:dyDescent="0.35">
       <c r="B20" s="40" t="s">
         <v>54</v>
       </c>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:22" ht="13" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:22" ht="12.75" x14ac:dyDescent="0.35">
       <c r="B21" s="17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="42" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:22" ht="38.25" x14ac:dyDescent="0.35">
       <c r="B22" s="37" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:22" ht="46" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:22" ht="46.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="39" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="13" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:22" ht="12.75" x14ac:dyDescent="0.35">
       <c r="V24" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' into Nolasco_Location_Choice"
This reverts commit 08626fa777cb9ba08560f4df04da59263fe86928, reversing
changes made to adda353bef58d3f5294999f2bdcff8277922ccd5.
</commit_message>
<xml_diff>
--- a/Artifacts/Team Meeting Log.xlsx
+++ b/Artifacts/Team Meeting Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cnkeng/Desktop/fall 2020 classes/Software Design/Software-Design/Artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979BBEC0-9D54-6B42-A4A1-50A82480D344}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272CA120-F5BE-5745-AC4B-A89E2E0EC163}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15360" yWindow="-28340" windowWidth="51200" windowHeight="28340" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20660" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
   </bookViews>
   <sheets>
     <sheet name="TeamF" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="91">
   <si>
     <t>Contact Info</t>
   </si>
@@ -313,40 +313,13 @@
   </si>
   <si>
     <t>Have coders close out their Jira tasks and expand upon the gameplay before next class.</t>
-  </si>
-  <si>
-    <t>Have everyone pull latest version of game from repo when it is done. Create stories for Sprint 2 during tomorrow's meeting.</t>
-  </si>
-  <si>
-    <t>Create stories for Sprint 2 and complete stand-up.</t>
-  </si>
-  <si>
-    <t>Check on the status of the game development,  make sure Jira is up-to-date, complete stand-up, and go over DoR &amp; DoD.</t>
-  </si>
-  <si>
-    <t>Checked on the status of the game development and ensured progress is reflected on Jira. Also completed daily stand-up and created our DoR &amp; DoD document.</t>
-  </si>
-  <si>
-    <t>Create a project timeline for Sprint 2 during tomorrow's meeting and create the retro slide as well.</t>
-  </si>
-  <si>
-    <t>We created our Sprint 2 stories and we went through our daily stand-up. We also marked our DoR &amp; DoD as done on Jira.</t>
-  </si>
-  <si>
-    <t>Retro w/ Prof. Vallone tonight.</t>
-  </si>
-  <si>
-    <t>Work on retro slide deck and discuss preparation for Sprint 2.</t>
-  </si>
-  <si>
-    <t>We created our retro slide deck, assigned speaking points, and formulated a Sprint 2 timeline.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -416,6 +389,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -624,14 +603,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -972,9 +951,9 @@
   </sheetPr>
   <dimension ref="A1:AX24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB15" sqref="AB15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y15" sqref="Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -999,10 +978,7 @@
     <col min="21" max="21" width="19" customWidth="1"/>
     <col min="22" max="22" width="18.6640625" customWidth="1"/>
     <col min="23" max="23" width="18.5" customWidth="1"/>
-    <col min="24" max="24" width="18.83203125" customWidth="1"/>
-    <col min="25" max="25" width="20.1640625" customWidth="1"/>
-    <col min="26" max="26" width="18.5" customWidth="1"/>
-    <col min="27" max="32" width="12.6640625" customWidth="1"/>
+    <col min="24" max="32" width="12.6640625" customWidth="1"/>
     <col min="33" max="37" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1288,15 +1264,9 @@
       <c r="W4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="X4" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y4" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z4" s="28" t="s">
-        <v>8</v>
-      </c>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="28"/>
+      <c r="Z4" s="28"/>
       <c r="AA4" s="28"/>
       <c r="AB4" s="28"/>
       <c r="AC4" s="28"/>
@@ -1348,14 +1318,14 @@
         <v>8</v>
       </c>
       <c r="O5" s="42"/>
-      <c r="P5" s="48"/>
+      <c r="P5" s="49"/>
       <c r="Q5" s="28" t="s">
         <v>8</v>
       </c>
       <c r="R5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="48"/>
+      <c r="S5" s="49"/>
       <c r="T5" s="28" t="s">
         <v>8</v>
       </c>
@@ -1366,15 +1336,9 @@
       <c r="W5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="X5" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y5" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z5" s="28" t="s">
-        <v>8</v>
-      </c>
+      <c r="X5" s="28"/>
+      <c r="Y5" s="28"/>
+      <c r="Z5" s="28"/>
       <c r="AA5" s="28"/>
       <c r="AB5" s="28"/>
       <c r="AC5" s="28"/>
@@ -1432,23 +1396,21 @@
       <c r="Q6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="R6" s="48"/>
+      <c r="R6" s="49"/>
       <c r="S6" s="28" t="s">
         <v>8</v>
       </c>
       <c r="T6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="U6" s="48"/>
+      <c r="U6" s="49"/>
       <c r="V6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="W6" s="48"/>
-      <c r="X6" s="48"/>
-      <c r="Y6" s="48"/>
-      <c r="Z6" s="28" t="s">
-        <v>8</v>
-      </c>
+      <c r="W6" s="49"/>
+      <c r="X6" s="28"/>
+      <c r="Y6" s="28"/>
+      <c r="Z6" s="28"/>
       <c r="AA6" s="28"/>
       <c r="AB6" s="28"/>
       <c r="AC6" s="28"/>
@@ -1506,7 +1468,7 @@
       <c r="Q7" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="R7" s="48"/>
+      <c r="R7" s="49"/>
       <c r="S7" s="28" t="s">
         <v>8</v>
       </c>
@@ -1518,15 +1480,9 @@
         <v>8</v>
       </c>
       <c r="W7" s="42"/>
-      <c r="X7" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y7" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z7" s="28" t="s">
-        <v>8</v>
-      </c>
+      <c r="X7" s="28"/>
+      <c r="Y7" s="28"/>
+      <c r="Z7" s="28"/>
       <c r="AA7" s="28"/>
       <c r="AB7" s="28"/>
       <c r="AC7" s="28"/>
@@ -1600,13 +1556,9 @@
       <c r="W8" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="X8" s="42"/>
-      <c r="Y8" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z8" s="28" t="s">
-        <v>8</v>
-      </c>
+      <c r="X8" s="28"/>
+      <c r="Y8" s="28"/>
+      <c r="Z8" s="28"/>
       <c r="AA8" s="28"/>
       <c r="AB8" s="28"/>
       <c r="AC8" s="28"/>
@@ -1665,30 +1617,24 @@
       <c r="P9" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="Q9" s="48"/>
+      <c r="Q9" s="49"/>
       <c r="R9" s="28" t="s">
         <v>8</v>
       </c>
       <c r="S9" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="T9" s="48"/>
+      <c r="T9" s="49"/>
       <c r="U9" s="28" t="s">
         <v>8</v>
       </c>
       <c r="V9" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="W9" s="48"/>
-      <c r="X9" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y9" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z9" s="28" t="s">
-        <v>8</v>
-      </c>
+      <c r="W9" s="49"/>
+      <c r="X9" s="28"/>
+      <c r="Y9" s="28"/>
+      <c r="Z9" s="28"/>
       <c r="AA9" s="28"/>
       <c r="AB9" s="28"/>
       <c r="AC9" s="28"/>
@@ -1744,39 +1690,27 @@
       <c r="O10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="P10" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q10" s="49" t="s">
+      <c r="P10" s="48"/>
+      <c r="Q10" s="50" t="s">
         <v>8</v>
       </c>
       <c r="R10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="S10" s="42" t="s">
-        <v>9</v>
-      </c>
+      <c r="S10" s="42"/>
       <c r="T10" s="28" t="s">
         <v>8</v>
       </c>
       <c r="U10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="V10" s="42" t="s">
-        <v>9</v>
-      </c>
+      <c r="V10" s="49"/>
       <c r="W10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="X10" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y10" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z10" s="28" t="s">
-        <v>8</v>
-      </c>
+      <c r="X10" s="28"/>
+      <c r="Y10" s="28"/>
+      <c r="Z10" s="28"/>
       <c r="AA10" s="28"/>
       <c r="AB10" s="28"/>
       <c r="AC10" s="28"/>
@@ -1859,15 +1793,9 @@
       <c r="W13" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="X13" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y13" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z13" s="18" t="s">
-        <v>98</v>
-      </c>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="18"/>
+      <c r="Z13" s="18"/>
       <c r="AA13" s="18"/>
       <c r="AB13" s="18"/>
       <c r="AC13" s="18"/>
@@ -1946,15 +1874,9 @@
       <c r="W14" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="X14" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y14" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="Z14" s="19" t="s">
-        <v>99</v>
-      </c>
+      <c r="X14" s="19"/>
+      <c r="Y14" s="19"/>
+      <c r="Z14" s="19"/>
       <c r="AA14" s="19"/>
       <c r="AB14" s="19"/>
       <c r="AC14" s="19"/>
@@ -2045,15 +1967,9 @@
       <c r="W15" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="X15" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y15" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z15" s="19" t="s">
-        <v>97</v>
-      </c>
+      <c r="X15" s="19"/>
+      <c r="Y15" s="19"/>
+      <c r="Z15" s="19"/>
       <c r="AA15" s="19"/>
       <c r="AB15" s="19"/>
       <c r="AC15" s="19"/>
@@ -2143,15 +2059,9 @@
       <c r="W16" s="20">
         <v>10</v>
       </c>
-      <c r="X16" s="20">
-        <v>40</v>
-      </c>
-      <c r="Y16" s="20">
-        <v>28</v>
-      </c>
-      <c r="Z16" s="20">
-        <v>35</v>
-      </c>
+      <c r="X16" s="20"/>
+      <c r="Y16" s="20"/>
+      <c r="Z16" s="20"/>
       <c r="AA16" s="20"/>
       <c r="AB16" s="20"/>
       <c r="AC16" s="20"/>

</xml_diff>

<commit_message>
Revert "Nolasco location choice"
</commit_message>
<xml_diff>
--- a/Artifacts/Team Meeting Log.xlsx
+++ b/Artifacts/Team Meeting Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cnkeng/Desktop/fall 2020 classes/Software Design/Software-Design/Artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272CA120-F5BE-5745-AC4B-A89E2E0EC163}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979BBEC0-9D54-6B42-A4A1-50A82480D344}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20660" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
+    <workbookView xWindow="-15360" yWindow="-28340" windowWidth="51200" windowHeight="28340" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
   </bookViews>
   <sheets>
     <sheet name="TeamF" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="100">
   <si>
     <t>Contact Info</t>
   </si>
@@ -313,13 +313,40 @@
   </si>
   <si>
     <t>Have coders close out their Jira tasks and expand upon the gameplay before next class.</t>
+  </si>
+  <si>
+    <t>Have everyone pull latest version of game from repo when it is done. Create stories for Sprint 2 during tomorrow's meeting.</t>
+  </si>
+  <si>
+    <t>Create stories for Sprint 2 and complete stand-up.</t>
+  </si>
+  <si>
+    <t>Check on the status of the game development,  make sure Jira is up-to-date, complete stand-up, and go over DoR &amp; DoD.</t>
+  </si>
+  <si>
+    <t>Checked on the status of the game development and ensured progress is reflected on Jira. Also completed daily stand-up and created our DoR &amp; DoD document.</t>
+  </si>
+  <si>
+    <t>Create a project timeline for Sprint 2 during tomorrow's meeting and create the retro slide as well.</t>
+  </si>
+  <si>
+    <t>We created our Sprint 2 stories and we went through our daily stand-up. We also marked our DoR &amp; DoD as done on Jira.</t>
+  </si>
+  <si>
+    <t>Retro w/ Prof. Vallone tonight.</t>
+  </si>
+  <si>
+    <t>Work on retro slide deck and discuss preparation for Sprint 2.</t>
+  </si>
+  <si>
+    <t>We created our retro slide deck, assigned speaking points, and formulated a Sprint 2 timeline.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -389,12 +416,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -603,14 +624,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -951,9 +972,9 @@
   </sheetPr>
   <dimension ref="A1:AX24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y15" sqref="Y15"/>
+    <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -978,7 +999,10 @@
     <col min="21" max="21" width="19" customWidth="1"/>
     <col min="22" max="22" width="18.6640625" customWidth="1"/>
     <col min="23" max="23" width="18.5" customWidth="1"/>
-    <col min="24" max="32" width="12.6640625" customWidth="1"/>
+    <col min="24" max="24" width="18.83203125" customWidth="1"/>
+    <col min="25" max="25" width="20.1640625" customWidth="1"/>
+    <col min="26" max="26" width="18.5" customWidth="1"/>
+    <col min="27" max="32" width="12.6640625" customWidth="1"/>
     <col min="33" max="37" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1264,9 +1288,15 @@
       <c r="W4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="X4" s="28"/>
-      <c r="Y4" s="28"/>
-      <c r="Z4" s="28"/>
+      <c r="X4" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y4" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z4" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AA4" s="28"/>
       <c r="AB4" s="28"/>
       <c r="AC4" s="28"/>
@@ -1318,14 +1348,14 @@
         <v>8</v>
       </c>
       <c r="O5" s="42"/>
-      <c r="P5" s="49"/>
+      <c r="P5" s="48"/>
       <c r="Q5" s="28" t="s">
         <v>8</v>
       </c>
       <c r="R5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="49"/>
+      <c r="S5" s="48"/>
       <c r="T5" s="28" t="s">
         <v>8</v>
       </c>
@@ -1336,9 +1366,15 @@
       <c r="W5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="X5" s="28"/>
-      <c r="Y5" s="28"/>
-      <c r="Z5" s="28"/>
+      <c r="X5" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y5" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z5" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AA5" s="28"/>
       <c r="AB5" s="28"/>
       <c r="AC5" s="28"/>
@@ -1396,21 +1432,23 @@
       <c r="Q6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="R6" s="49"/>
+      <c r="R6" s="48"/>
       <c r="S6" s="28" t="s">
         <v>8</v>
       </c>
       <c r="T6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="U6" s="49"/>
+      <c r="U6" s="48"/>
       <c r="V6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="W6" s="49"/>
-      <c r="X6" s="28"/>
-      <c r="Y6" s="28"/>
-      <c r="Z6" s="28"/>
+      <c r="W6" s="48"/>
+      <c r="X6" s="48"/>
+      <c r="Y6" s="48"/>
+      <c r="Z6" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AA6" s="28"/>
       <c r="AB6" s="28"/>
       <c r="AC6" s="28"/>
@@ -1468,7 +1506,7 @@
       <c r="Q7" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="R7" s="49"/>
+      <c r="R7" s="48"/>
       <c r="S7" s="28" t="s">
         <v>8</v>
       </c>
@@ -1480,9 +1518,15 @@
         <v>8</v>
       </c>
       <c r="W7" s="42"/>
-      <c r="X7" s="28"/>
-      <c r="Y7" s="28"/>
-      <c r="Z7" s="28"/>
+      <c r="X7" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y7" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z7" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AA7" s="28"/>
       <c r="AB7" s="28"/>
       <c r="AC7" s="28"/>
@@ -1556,9 +1600,13 @@
       <c r="W8" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="X8" s="28"/>
-      <c r="Y8" s="28"/>
-      <c r="Z8" s="28"/>
+      <c r="X8" s="42"/>
+      <c r="Y8" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z8" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AA8" s="28"/>
       <c r="AB8" s="28"/>
       <c r="AC8" s="28"/>
@@ -1617,24 +1665,30 @@
       <c r="P9" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="Q9" s="49"/>
+      <c r="Q9" s="48"/>
       <c r="R9" s="28" t="s">
         <v>8</v>
       </c>
       <c r="S9" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="T9" s="49"/>
+      <c r="T9" s="48"/>
       <c r="U9" s="28" t="s">
         <v>8</v>
       </c>
       <c r="V9" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="W9" s="49"/>
-      <c r="X9" s="28"/>
-      <c r="Y9" s="28"/>
-      <c r="Z9" s="28"/>
+      <c r="W9" s="48"/>
+      <c r="X9" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y9" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z9" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AA9" s="28"/>
       <c r="AB9" s="28"/>
       <c r="AC9" s="28"/>
@@ -1690,27 +1744,39 @@
       <c r="O10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="P10" s="48"/>
-      <c r="Q10" s="50" t="s">
+      <c r="P10" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q10" s="49" t="s">
         <v>8</v>
       </c>
       <c r="R10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="S10" s="42"/>
+      <c r="S10" s="42" t="s">
+        <v>9</v>
+      </c>
       <c r="T10" s="28" t="s">
         <v>8</v>
       </c>
       <c r="U10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="V10" s="49"/>
+      <c r="V10" s="42" t="s">
+        <v>9</v>
+      </c>
       <c r="W10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="X10" s="28"/>
-      <c r="Y10" s="28"/>
-      <c r="Z10" s="28"/>
+      <c r="X10" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y10" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z10" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AA10" s="28"/>
       <c r="AB10" s="28"/>
       <c r="AC10" s="28"/>
@@ -1793,9 +1859,15 @@
       <c r="W13" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="18"/>
+      <c r="X13" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y13" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z13" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="AA13" s="18"/>
       <c r="AB13" s="18"/>
       <c r="AC13" s="18"/>
@@ -1874,9 +1946,15 @@
       <c r="W14" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="X14" s="19"/>
-      <c r="Y14" s="19"/>
-      <c r="Z14" s="19"/>
+      <c r="X14" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y14" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z14" s="19" t="s">
+        <v>99</v>
+      </c>
       <c r="AA14" s="19"/>
       <c r="AB14" s="19"/>
       <c r="AC14" s="19"/>
@@ -1967,9 +2045,15 @@
       <c r="W15" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="X15" s="19"/>
-      <c r="Y15" s="19"/>
-      <c r="Z15" s="19"/>
+      <c r="X15" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y15" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z15" s="19" t="s">
+        <v>97</v>
+      </c>
       <c r="AA15" s="19"/>
       <c r="AB15" s="19"/>
       <c r="AC15" s="19"/>
@@ -2059,9 +2143,15 @@
       <c r="W16" s="20">
         <v>10</v>
       </c>
-      <c r="X16" s="20"/>
-      <c r="Y16" s="20"/>
-      <c r="Z16" s="20"/>
+      <c r="X16" s="20">
+        <v>40</v>
+      </c>
+      <c r="Y16" s="20">
+        <v>28</v>
+      </c>
+      <c r="Z16" s="20">
+        <v>35</v>
+      </c>
       <c r="AA16" s="20"/>
       <c r="AB16" s="20"/>
       <c r="AC16" s="20"/>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' into Nolasco_Location_Choice""
This reverts commit 5133b8a9d70e8980983b45195a62b7b7a39c88e7.
</commit_message>
<xml_diff>
--- a/Artifacts/Team Meeting Log.xlsx
+++ b/Artifacts/Team Meeting Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cnkeng/Desktop/fall 2020 classes/Software Design/Software-Design/Artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272CA120-F5BE-5745-AC4B-A89E2E0EC163}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979BBEC0-9D54-6B42-A4A1-50A82480D344}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20660" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
+    <workbookView xWindow="-15360" yWindow="-28340" windowWidth="51200" windowHeight="28340" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
   </bookViews>
   <sheets>
     <sheet name="TeamF" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="100">
   <si>
     <t>Contact Info</t>
   </si>
@@ -313,13 +313,40 @@
   </si>
   <si>
     <t>Have coders close out their Jira tasks and expand upon the gameplay before next class.</t>
+  </si>
+  <si>
+    <t>Have everyone pull latest version of game from repo when it is done. Create stories for Sprint 2 during tomorrow's meeting.</t>
+  </si>
+  <si>
+    <t>Create stories for Sprint 2 and complete stand-up.</t>
+  </si>
+  <si>
+    <t>Check on the status of the game development,  make sure Jira is up-to-date, complete stand-up, and go over DoR &amp; DoD.</t>
+  </si>
+  <si>
+    <t>Checked on the status of the game development and ensured progress is reflected on Jira. Also completed daily stand-up and created our DoR &amp; DoD document.</t>
+  </si>
+  <si>
+    <t>Create a project timeline for Sprint 2 during tomorrow's meeting and create the retro slide as well.</t>
+  </si>
+  <si>
+    <t>We created our Sprint 2 stories and we went through our daily stand-up. We also marked our DoR &amp; DoD as done on Jira.</t>
+  </si>
+  <si>
+    <t>Retro w/ Prof. Vallone tonight.</t>
+  </si>
+  <si>
+    <t>Work on retro slide deck and discuss preparation for Sprint 2.</t>
+  </si>
+  <si>
+    <t>We created our retro slide deck, assigned speaking points, and formulated a Sprint 2 timeline.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -389,12 +416,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -603,14 +624,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -951,9 +972,9 @@
   </sheetPr>
   <dimension ref="A1:AX24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="116" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y15" sqref="Y15"/>
+    <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -978,7 +999,10 @@
     <col min="21" max="21" width="19" customWidth="1"/>
     <col min="22" max="22" width="18.6640625" customWidth="1"/>
     <col min="23" max="23" width="18.5" customWidth="1"/>
-    <col min="24" max="32" width="12.6640625" customWidth="1"/>
+    <col min="24" max="24" width="18.83203125" customWidth="1"/>
+    <col min="25" max="25" width="20.1640625" customWidth="1"/>
+    <col min="26" max="26" width="18.5" customWidth="1"/>
+    <col min="27" max="32" width="12.6640625" customWidth="1"/>
     <col min="33" max="37" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1264,9 +1288,15 @@
       <c r="W4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="X4" s="28"/>
-      <c r="Y4" s="28"/>
-      <c r="Z4" s="28"/>
+      <c r="X4" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y4" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z4" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AA4" s="28"/>
       <c r="AB4" s="28"/>
       <c r="AC4" s="28"/>
@@ -1318,14 +1348,14 @@
         <v>8</v>
       </c>
       <c r="O5" s="42"/>
-      <c r="P5" s="49"/>
+      <c r="P5" s="48"/>
       <c r="Q5" s="28" t="s">
         <v>8</v>
       </c>
       <c r="R5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="49"/>
+      <c r="S5" s="48"/>
       <c r="T5" s="28" t="s">
         <v>8</v>
       </c>
@@ -1336,9 +1366,15 @@
       <c r="W5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="X5" s="28"/>
-      <c r="Y5" s="28"/>
-      <c r="Z5" s="28"/>
+      <c r="X5" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y5" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z5" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AA5" s="28"/>
       <c r="AB5" s="28"/>
       <c r="AC5" s="28"/>
@@ -1396,21 +1432,23 @@
       <c r="Q6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="R6" s="49"/>
+      <c r="R6" s="48"/>
       <c r="S6" s="28" t="s">
         <v>8</v>
       </c>
       <c r="T6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="U6" s="49"/>
+      <c r="U6" s="48"/>
       <c r="V6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="W6" s="49"/>
-      <c r="X6" s="28"/>
-      <c r="Y6" s="28"/>
-      <c r="Z6" s="28"/>
+      <c r="W6" s="48"/>
+      <c r="X6" s="48"/>
+      <c r="Y6" s="48"/>
+      <c r="Z6" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AA6" s="28"/>
       <c r="AB6" s="28"/>
       <c r="AC6" s="28"/>
@@ -1468,7 +1506,7 @@
       <c r="Q7" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="R7" s="49"/>
+      <c r="R7" s="48"/>
       <c r="S7" s="28" t="s">
         <v>8</v>
       </c>
@@ -1480,9 +1518,15 @@
         <v>8</v>
       </c>
       <c r="W7" s="42"/>
-      <c r="X7" s="28"/>
-      <c r="Y7" s="28"/>
-      <c r="Z7" s="28"/>
+      <c r="X7" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y7" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z7" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AA7" s="28"/>
       <c r="AB7" s="28"/>
       <c r="AC7" s="28"/>
@@ -1556,9 +1600,13 @@
       <c r="W8" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="X8" s="28"/>
-      <c r="Y8" s="28"/>
-      <c r="Z8" s="28"/>
+      <c r="X8" s="42"/>
+      <c r="Y8" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z8" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AA8" s="28"/>
       <c r="AB8" s="28"/>
       <c r="AC8" s="28"/>
@@ -1617,24 +1665,30 @@
       <c r="P9" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="Q9" s="49"/>
+      <c r="Q9" s="48"/>
       <c r="R9" s="28" t="s">
         <v>8</v>
       </c>
       <c r="S9" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="T9" s="49"/>
+      <c r="T9" s="48"/>
       <c r="U9" s="28" t="s">
         <v>8</v>
       </c>
       <c r="V9" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="W9" s="49"/>
-      <c r="X9" s="28"/>
-      <c r="Y9" s="28"/>
-      <c r="Z9" s="28"/>
+      <c r="W9" s="48"/>
+      <c r="X9" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y9" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z9" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AA9" s="28"/>
       <c r="AB9" s="28"/>
       <c r="AC9" s="28"/>
@@ -1690,27 +1744,39 @@
       <c r="O10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="P10" s="48"/>
-      <c r="Q10" s="50" t="s">
+      <c r="P10" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q10" s="49" t="s">
         <v>8</v>
       </c>
       <c r="R10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="S10" s="42"/>
+      <c r="S10" s="42" t="s">
+        <v>9</v>
+      </c>
       <c r="T10" s="28" t="s">
         <v>8</v>
       </c>
       <c r="U10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="V10" s="49"/>
+      <c r="V10" s="42" t="s">
+        <v>9</v>
+      </c>
       <c r="W10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="X10" s="28"/>
-      <c r="Y10" s="28"/>
-      <c r="Z10" s="28"/>
+      <c r="X10" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y10" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z10" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AA10" s="28"/>
       <c r="AB10" s="28"/>
       <c r="AC10" s="28"/>
@@ -1793,9 +1859,15 @@
       <c r="W13" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="18"/>
+      <c r="X13" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y13" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z13" s="18" t="s">
+        <v>98</v>
+      </c>
       <c r="AA13" s="18"/>
       <c r="AB13" s="18"/>
       <c r="AC13" s="18"/>
@@ -1874,9 +1946,15 @@
       <c r="W14" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="X14" s="19"/>
-      <c r="Y14" s="19"/>
-      <c r="Z14" s="19"/>
+      <c r="X14" s="50" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y14" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z14" s="19" t="s">
+        <v>99</v>
+      </c>
       <c r="AA14" s="19"/>
       <c r="AB14" s="19"/>
       <c r="AC14" s="19"/>
@@ -1967,9 +2045,15 @@
       <c r="W15" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="X15" s="19"/>
-      <c r="Y15" s="19"/>
-      <c r="Z15" s="19"/>
+      <c r="X15" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y15" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z15" s="19" t="s">
+        <v>97</v>
+      </c>
       <c r="AA15" s="19"/>
       <c r="AB15" s="19"/>
       <c r="AC15" s="19"/>
@@ -2059,9 +2143,15 @@
       <c r="W16" s="20">
         <v>10</v>
       </c>
-      <c r="X16" s="20"/>
-      <c r="Y16" s="20"/>
-      <c r="Z16" s="20"/>
+      <c r="X16" s="20">
+        <v>40</v>
+      </c>
+      <c r="Y16" s="20">
+        <v>28</v>
+      </c>
+      <c r="Z16" s="20">
+        <v>35</v>
+      </c>
       <c r="AA16" s="20"/>
       <c r="AB16" s="20"/>
       <c r="AC16" s="20"/>

</xml_diff>

<commit_message>
sprint 2 review and attendance log
</commit_message>
<xml_diff>
--- a/Artifacts/Team Meeting Log.xlsx
+++ b/Artifacts/Team Meeting Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cnkeng/Desktop/fall 2020 classes/Software Design/Software-Design/Artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8BB9A4-6084-2D4B-A3F9-C2D0F0EE7691}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877DE9B3-555B-5C4C-9E99-C26DD2F6CA3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7420" yWindow="-28340" windowWidth="51200" windowHeight="28340" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
+    <workbookView xWindow="-8080" yWindow="-28340" windowWidth="51200" windowHeight="28340" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
   </bookViews>
   <sheets>
     <sheet name="TeamF" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="111">
   <si>
     <t>Contact Info</t>
   </si>
@@ -361,6 +361,18 @@
   </si>
   <si>
     <t>Sprint Planning</t>
+  </si>
+  <si>
+    <t>Prepare for tomorrow's meeting.</t>
+  </si>
+  <si>
+    <t>Move some stories from Sprint 2 to Sprint 3, and plan out what we will be doing for the next sprint. Also, we will be doing Pointing Poker.</t>
+  </si>
+  <si>
+    <t>Checked on the status of the game and the bugs, and created the slide deck in preparation for tomorrow's demo.</t>
+  </si>
+  <si>
+    <t>Make sure all bugs fixed for demo tomorrow, all changes are pushed and merged into master, and we will also work on some of our Sprint 2 planning.</t>
   </si>
 </sst>
 </file>
@@ -534,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -663,12 +675,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -677,6 +683,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1000,7 +1015,7 @@
   <dimension ref="A1:AY24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AF15" sqref="AF15"/>
     </sheetView>
   </sheetViews>
@@ -1032,46 +1047,48 @@
     <col min="27" max="27" width="17.1640625" customWidth="1"/>
     <col min="28" max="28" width="16.6640625" customWidth="1"/>
     <col min="29" max="30" width="20.33203125" customWidth="1"/>
-    <col min="31" max="33" width="12.6640625" customWidth="1"/>
+    <col min="31" max="31" width="19.6640625" customWidth="1"/>
+    <col min="32" max="32" width="20.5" customWidth="1"/>
+    <col min="33" max="33" width="12.6640625" customWidth="1"/>
     <col min="34" max="38" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
       <c r="J1" s="26"/>
       <c r="K1" s="26"/>
     </row>
     <row r="2" spans="1:51" s="23" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="58" t="s">
+      <c r="C2" s="55"/>
+      <c r="D2" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58" t="s">
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="58"/>
-      <c r="S2" s="58"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
       <c r="T2" s="53" t="s">
         <v>1</v>
       </c>
@@ -1343,8 +1360,12 @@
       <c r="AD4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AE4" s="28"/>
-      <c r="AF4" s="28"/>
+      <c r="AE4" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF4" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AG4" s="28"/>
       <c r="AH4" s="28"/>
       <c r="AI4" s="28"/>
@@ -1428,7 +1449,9 @@
       <c r="AD5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AE5" s="28"/>
+      <c r="AE5" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AF5" s="28"/>
       <c r="AG5" s="28"/>
       <c r="AH5" s="28"/>
@@ -1505,7 +1528,9 @@
       </c>
       <c r="AC6" s="48"/>
       <c r="AD6" s="48"/>
-      <c r="AE6" s="28"/>
+      <c r="AE6" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AF6" s="28"/>
       <c r="AG6" s="28"/>
       <c r="AH6" s="28"/>
@@ -1592,7 +1617,7 @@
       <c r="AD7" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AE7" s="28"/>
+      <c r="AE7" s="42"/>
       <c r="AF7" s="28"/>
       <c r="AG7" s="28"/>
       <c r="AH7" s="28"/>
@@ -1679,7 +1704,9 @@
       <c r="AD8" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AE8" s="28"/>
+      <c r="AE8" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AF8" s="28"/>
       <c r="AG8" s="28"/>
       <c r="AH8" s="28"/>
@@ -1768,7 +1795,9 @@
       <c r="AD9" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AE9" s="28"/>
+      <c r="AE9" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AF9" s="28"/>
       <c r="AG9" s="28"/>
       <c r="AH9" s="28"/>
@@ -1865,7 +1894,9 @@
       <c r="AD10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AE10" s="28"/>
+      <c r="AE10" s="57" t="s">
+        <v>8</v>
+      </c>
       <c r="AF10" s="28"/>
       <c r="AG10" s="28"/>
       <c r="AH10" s="28"/>
@@ -1965,8 +1996,12 @@
       <c r="AD13" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="AE13" s="18"/>
-      <c r="AF13" s="18"/>
+      <c r="AE13" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF13" s="18" t="s">
+        <v>108</v>
+      </c>
       <c r="AG13" s="18"/>
       <c r="AH13" s="18"/>
       <c r="AI13" s="18"/>
@@ -2061,13 +2096,15 @@
       <c r="AD14" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="AE14" s="51"/>
+      <c r="AE14" s="51" t="s">
+        <v>109</v>
+      </c>
       <c r="AF14" s="19"/>
       <c r="AG14" s="19"/>
       <c r="AH14" s="19"/>
       <c r="AI14" s="19"/>
-      <c r="AJ14" s="54"/>
-      <c r="AK14" s="55"/>
+      <c r="AJ14" s="58"/>
+      <c r="AK14" s="59"/>
       <c r="AL14" s="19"/>
       <c r="AM14" s="19"/>
       <c r="AN14" s="6"/>
@@ -2169,7 +2206,9 @@
       <c r="AD15" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="AE15" s="51"/>
+      <c r="AE15" s="51" t="s">
+        <v>107</v>
+      </c>
       <c r="AF15" s="19"/>
       <c r="AG15" s="19"/>
       <c r="AH15" s="19"/>
@@ -2276,7 +2315,9 @@
       <c r="AD16" s="20">
         <v>65</v>
       </c>
-      <c r="AE16" s="20"/>
+      <c r="AE16" s="20">
+        <v>30</v>
+      </c>
       <c r="AF16" s="20"/>
       <c r="AG16" s="20"/>
       <c r="AH16" s="20"/>
@@ -2329,9 +2370,8 @@
       <c r="V24" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="8">
     <mergeCell ref="AM2:AQ2"/>
-    <mergeCell ref="AJ14:AK14"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:H2"/>

</xml_diff>

<commit_message>
attendance log and sprint 3 review
</commit_message>
<xml_diff>
--- a/Artifacts/Team Meeting Log.xlsx
+++ b/Artifacts/Team Meeting Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cnkeng/Desktop/fall 2020 classes/Software Design/Software-Design/Artifacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F50526F-FADF-FC40-9F44-07268ABE29BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FED5DAF-BADD-6249-AB0A-5888844D7F33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-9100" yWindow="-28340" windowWidth="51200" windowHeight="28340" xr2:uid="{B69BAA51-2B07-4930-841B-9107909D754E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="126">
   <si>
     <t>Contact Info</t>
   </si>
@@ -412,6 +412,12 @@
   </si>
   <si>
     <t>Closed out Sprint 3.</t>
+  </si>
+  <si>
+    <t>Retro &amp; demo prepared for tonight, discuss issues with other people downloading the game, and possibly Pointing Poker for Sprint 4 stories.</t>
+  </si>
+  <si>
+    <t>Prepared the Sprint 3 Review and demo for tonight, and tried to troubleshoot the GameJolt permissions issue.</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1054,7 @@
   <dimension ref="A1:AZ24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AG1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="AF1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AN14" sqref="AN14"/>
     </sheetView>
   </sheetViews>
@@ -1087,7 +1093,7 @@
     <col min="36" max="36" width="20.6640625" customWidth="1"/>
     <col min="37" max="37" width="22.5" customWidth="1"/>
     <col min="38" max="38" width="21.5" customWidth="1"/>
-    <col min="39" max="39" width="12" customWidth="1"/>
+    <col min="39" max="39" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1423,7 +1429,9 @@
       <c r="AL4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AM4" s="28"/>
+      <c r="AM4" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AN4" s="29"/>
     </row>
     <row r="5" spans="1:52" ht="13" x14ac:dyDescent="0.15">
@@ -1521,7 +1529,9 @@
       <c r="AL5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AM5" s="28"/>
+      <c r="AM5" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AN5" s="29"/>
     </row>
     <row r="6" spans="1:52" ht="13" x14ac:dyDescent="0.15">
@@ -1601,7 +1611,9 @@
       <c r="AJ6" s="48"/>
       <c r="AK6" s="38"/>
       <c r="AL6" s="42"/>
-      <c r="AM6" s="28"/>
+      <c r="AM6" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AN6" s="29"/>
     </row>
     <row r="7" spans="1:52" ht="14" x14ac:dyDescent="0.15">
@@ -1703,7 +1715,7 @@
       <c r="AL7" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AM7" s="28"/>
+      <c r="AM7" s="42"/>
       <c r="AN7" s="29"/>
     </row>
     <row r="8" spans="1:52" ht="13" x14ac:dyDescent="0.15">
@@ -1803,7 +1815,9 @@
       <c r="AL8" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AM8" s="28"/>
+      <c r="AM8" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AN8" s="29"/>
     </row>
     <row r="9" spans="1:52" ht="13" x14ac:dyDescent="0.15">
@@ -1905,7 +1919,9 @@
       <c r="AL9" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AM9" s="28"/>
+      <c r="AM9" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="AN9" s="29"/>
     </row>
     <row r="10" spans="1:52" ht="14" x14ac:dyDescent="0.15">
@@ -2017,7 +2033,9 @@
       <c r="AL10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AM10" s="28"/>
+      <c r="AM10" s="42" t="s">
+        <v>9</v>
+      </c>
       <c r="AN10" s="29"/>
     </row>
     <row r="11" spans="1:52" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2137,7 +2155,9 @@
       <c r="AL13" s="52" t="s">
         <v>122</v>
       </c>
-      <c r="AM13" s="18"/>
+      <c r="AM13" s="18" t="s">
+        <v>124</v>
+      </c>
       <c r="AN13" s="18"/>
     </row>
     <row r="14" spans="1:52" s="5" customFormat="1" ht="259" customHeight="1" x14ac:dyDescent="0.15">
@@ -2250,7 +2270,9 @@
       <c r="AL14" s="52" t="s">
         <v>123</v>
       </c>
-      <c r="AM14" s="19"/>
+      <c r="AM14" s="19" t="s">
+        <v>125</v>
+      </c>
       <c r="AN14" s="19"/>
       <c r="AO14" s="6"/>
       <c r="AP14" s="6"/>
@@ -2375,7 +2397,9 @@
       <c r="AL15" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="AM15" s="19"/>
+      <c r="AM15" s="19" t="s">
+        <v>121</v>
+      </c>
       <c r="AN15" s="19"/>
       <c r="AO15" s="7"/>
       <c r="AP15" s="7"/>
@@ -2499,7 +2523,9 @@
       <c r="AL16" s="20">
         <v>24</v>
       </c>
-      <c r="AM16" s="20"/>
+      <c r="AM16" s="20">
+        <v>40</v>
+      </c>
       <c r="AN16" s="20"/>
       <c r="AO16" s="44"/>
       <c r="AP16" s="44"/>

</xml_diff>